<commit_message>
Bump log4j version (for a security patch).
</commit_message>
<xml_diff>
--- a/Lucene_8_tokenize_analyze_filter.xlsx
+++ b/Lucene_8_tokenize_analyze_filter.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="189" documentId="8_{723A6461-7707-4E93-A563-5651A7972479}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B7C5A57D-2DAE-43A6-B0F2-3A6F5D636F4A}"/>
+  <xr:revisionPtr revIDLastSave="191" documentId="8_{723A6461-7707-4E93-A563-5651A7972479}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D9AC81EF-9A6F-4ED2-AAEE-A6765938691F}"/>
   <bookViews>
     <workbookView xWindow="1065" yWindow="495" windowWidth="21060" windowHeight="19620" activeTab="3" xr2:uid="{B0E7D34D-E2E7-448C-9EE0-FD93A17E1333}"/>
   </bookViews>
@@ -3786,8 +3786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD447F74-1863-49FF-8C3A-67503193C826}">
   <dimension ref="B1:F129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>